<commit_message>
Updated sentiment data stats
</commit_message>
<xml_diff>
--- a/data_exploration/acl/tables/basic_stats_sentiment_mbert.xlsx
+++ b/data_exploration/acl/tables/basic_stats_sentiment_mbert.xlsx
@@ -555,58 +555,58 @@
         <v>19</v>
       </c>
       <c r="B2">
-        <v>4939</v>
+        <v>6444</v>
       </c>
       <c r="C2">
-        <v>705</v>
+        <v>772</v>
       </c>
       <c r="D2">
-        <v>1412</v>
+        <v>1490</v>
       </c>
       <c r="E2">
-        <v>44.76918404535331</v>
+        <v>81.66977032898821</v>
       </c>
       <c r="F2">
-        <v>44.06666666666667</v>
+        <v>85.22020725388602</v>
       </c>
       <c r="G2">
-        <v>45.53611898016997</v>
+        <v>92.78120805369127</v>
       </c>
       <c r="H2">
-        <v>2292</v>
+        <v>3460</v>
       </c>
       <c r="I2">
-        <v>1.036564683535717</v>
+        <v>0.6574447062400244</v>
       </c>
       <c r="J2">
-        <v>1408</v>
+        <v>2510</v>
       </c>
       <c r="K2">
-        <v>4.532140213087843</v>
+        <v>3.815169478644171</v>
       </c>
       <c r="L2">
-        <v>1733</v>
+        <v>2766</v>
       </c>
       <c r="M2">
-        <v>2.695304602080968</v>
+        <v>2.000810161743005</v>
       </c>
       <c r="N2">
-        <v>194</v>
+        <v>1851</v>
       </c>
       <c r="O2">
-        <v>0.08773715035162699</v>
+        <v>0.3517139165463252</v>
       </c>
       <c r="P2">
-        <v>22</v>
+        <v>230</v>
       </c>
       <c r="Q2">
-        <v>0.07081469082949754</v>
+        <v>0.3495972032223743</v>
       </c>
       <c r="R2">
-        <v>62</v>
+        <v>405</v>
       </c>
       <c r="S2">
-        <v>0.09642751605829199</v>
+        <v>0.2929602731402448</v>
       </c>
     </row>
     <row r="3" spans="1:19">
@@ -791,58 +791,58 @@
         <v>23</v>
       </c>
       <c r="B6">
-        <v>462</v>
+        <v>5936</v>
       </c>
       <c r="C6">
-        <v>66</v>
+        <v>383</v>
       </c>
       <c r="D6">
-        <v>133</v>
+        <v>767</v>
       </c>
       <c r="E6">
-        <v>59.61904761904762</v>
+        <v>155.2505053908356</v>
       </c>
       <c r="F6">
-        <v>58.27272727272727</v>
+        <v>96.18537859007833</v>
       </c>
       <c r="G6">
-        <v>56.81203007518797</v>
+        <v>96.77444589308996</v>
       </c>
       <c r="H6">
-        <v>857</v>
+        <v>1097</v>
       </c>
       <c r="I6">
-        <v>3.111385419692129</v>
+        <v>0.1190363804259484</v>
       </c>
       <c r="J6">
-        <v>348</v>
+        <v>785</v>
       </c>
       <c r="K6">
-        <v>9.048361934477379</v>
+        <v>2.13089388962784</v>
       </c>
       <c r="L6">
-        <v>510</v>
+        <v>990</v>
       </c>
       <c r="M6">
-        <v>6.749602964531498</v>
+        <v>1.333764449114865</v>
       </c>
       <c r="N6">
-        <v>53</v>
+        <v>140</v>
       </c>
       <c r="O6">
-        <v>0.1924194016845774</v>
+        <v>0.01519151618927327</v>
       </c>
       <c r="P6">
-        <v>5</v>
+        <v>32</v>
       </c>
       <c r="Q6">
-        <v>0.1300052002080083</v>
+        <v>0.08686446429056163</v>
       </c>
       <c r="R6">
-        <v>10</v>
+        <v>73</v>
       </c>
       <c r="S6">
-        <v>0.1323451561672843</v>
+        <v>0.09834828766200523</v>
       </c>
     </row>
     <row r="7" spans="1:19">
@@ -1086,58 +1086,58 @@
         <v>28</v>
       </c>
       <c r="B11">
-        <v>11881</v>
+        <v>7926</v>
       </c>
       <c r="C11">
-        <v>1697</v>
+        <v>1132</v>
       </c>
       <c r="D11">
-        <v>3396</v>
+        <v>2266</v>
       </c>
       <c r="E11">
-        <v>23.65002945879976</v>
+        <v>52.47451425687611</v>
       </c>
       <c r="F11">
-        <v>24.07424867413082</v>
+        <v>52.47614840989399</v>
       </c>
       <c r="G11">
-        <v>23.38604240282686</v>
+        <v>51.96028243601059</v>
       </c>
       <c r="H11">
-        <v>1816</v>
+        <v>1862</v>
       </c>
       <c r="I11">
-        <v>0.646295544973771</v>
+        <v>0.4476897812763727</v>
       </c>
       <c r="J11">
-        <v>1236</v>
+        <v>1333</v>
       </c>
       <c r="K11">
-        <v>3.025407548832427</v>
+        <v>2.243994411056681</v>
       </c>
       <c r="L11">
-        <v>1483</v>
+        <v>1557</v>
       </c>
       <c r="M11">
-        <v>1.867311348669714</v>
+        <v>1.3223828370505</v>
       </c>
       <c r="N11">
-        <v>286</v>
+        <v>0</v>
       </c>
       <c r="O11">
-        <v>0.1017844305410234</v>
+        <v>0</v>
       </c>
       <c r="P11">
-        <v>35</v>
+        <v>0</v>
       </c>
       <c r="Q11">
-        <v>0.08567092573554609</v>
+        <v>0</v>
       </c>
       <c r="R11">
-        <v>70</v>
+        <v>0</v>
       </c>
       <c r="S11">
-        <v>0.08814011760409977</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:19">
@@ -1145,58 +1145,58 @@
         <v>29</v>
       </c>
       <c r="B12">
-        <v>1355</v>
+        <v>4432</v>
       </c>
       <c r="C12">
-        <v>199</v>
+        <v>633</v>
       </c>
       <c r="D12">
-        <v>397</v>
+        <v>1267</v>
       </c>
       <c r="E12">
-        <v>93.26125461254613</v>
+        <v>29.50676895306859</v>
       </c>
       <c r="F12">
-        <v>95.31658291457286</v>
+        <v>26.64296998420221</v>
       </c>
       <c r="G12">
-        <v>92.48866498740554</v>
+        <v>28.53433307024467</v>
       </c>
       <c r="H12">
-        <v>1704</v>
+        <v>2118</v>
       </c>
       <c r="I12">
-        <v>1.348431973031361</v>
+        <v>1.619587991496781</v>
       </c>
       <c r="J12">
-        <v>1215</v>
+        <v>1334</v>
       </c>
       <c r="K12">
-        <v>6.405525094896667</v>
+        <v>7.909872517047139</v>
       </c>
       <c r="L12">
-        <v>1320</v>
+        <v>1592</v>
       </c>
       <c r="M12">
-        <v>3.59496704613541</v>
+        <v>4.403507316128676</v>
       </c>
       <c r="N12">
-        <v>15</v>
+        <v>36</v>
       </c>
       <c r="O12">
-        <v>0.0118699997626</v>
+        <v>0.02752840778748069</v>
       </c>
       <c r="P12">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="Q12">
-        <v>0.01054407423028258</v>
+        <v>0.04743551734361103</v>
       </c>
       <c r="R12">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="S12">
-        <v>0.005446919766871834</v>
+        <v>0.01659613310098747</v>
       </c>
     </row>
     <row r="13" spans="1:19">
@@ -1263,58 +1263,58 @@
         <v>31</v>
       </c>
       <c r="B14">
-        <v>3237</v>
+        <v>36000</v>
       </c>
       <c r="C14">
-        <v>463</v>
+        <v>1333</v>
       </c>
       <c r="D14">
-        <v>926</v>
+        <v>2667</v>
       </c>
       <c r="E14">
-        <v>44.17763361136855</v>
+        <v>26.3625</v>
       </c>
       <c r="F14">
-        <v>39.24190064794816</v>
+        <v>27.47861965491373</v>
       </c>
       <c r="G14">
-        <v>43.03887688984882</v>
+        <v>25.92688413948256</v>
       </c>
       <c r="H14">
-        <v>445</v>
+        <v>1095</v>
       </c>
       <c r="I14">
-        <v>0.3111822828891702</v>
+        <v>0.115378536431168</v>
       </c>
       <c r="J14">
-        <v>507</v>
+        <v>575</v>
       </c>
       <c r="K14">
-        <v>2.790467279432</v>
+        <v>1.569794425182232</v>
       </c>
       <c r="L14">
-        <v>448</v>
+        <v>521</v>
       </c>
       <c r="M14">
-        <v>1.124102975861896</v>
+        <v>0.7534672509291799</v>
       </c>
       <c r="N14">
-        <v>608</v>
+        <v>14830</v>
       </c>
       <c r="O14">
-        <v>0.4251659056103718</v>
+        <v>1.562615246825773</v>
       </c>
       <c r="P14">
-        <v>42</v>
+        <v>588</v>
       </c>
       <c r="Q14">
-        <v>0.2311629698937751</v>
+        <v>1.605285429577657</v>
       </c>
       <c r="R14">
-        <v>184</v>
+        <v>1140</v>
       </c>
       <c r="S14">
-        <v>0.4616851508004215</v>
+        <v>1.648661547138704</v>
       </c>
     </row>
     <row r="15" spans="1:19">
@@ -1381,52 +1381,52 @@
         <v>33</v>
       </c>
       <c r="B16">
-        <v>915</v>
+        <v>4486</v>
       </c>
       <c r="C16">
-        <v>21</v>
+        <v>105</v>
       </c>
       <c r="D16">
-        <v>116</v>
+        <v>211</v>
       </c>
       <c r="E16">
-        <v>23.13879781420765</v>
+        <v>56.87895675434686</v>
       </c>
       <c r="F16">
-        <v>21.19047619047619</v>
+        <v>23.37142857142857</v>
       </c>
       <c r="G16">
-        <v>21.89655172413793</v>
+        <v>22.62085308056872</v>
       </c>
       <c r="H16">
-        <v>899</v>
+        <v>1597</v>
       </c>
       <c r="I16">
-        <v>4.246174192329492</v>
+        <v>0.6258842525640875</v>
       </c>
       <c r="J16">
-        <v>190</v>
+        <v>555</v>
       </c>
       <c r="K16">
-        <v>42.69662921348314</v>
+        <v>22.6161369193154</v>
       </c>
       <c r="L16">
-        <v>507</v>
+        <v>690</v>
       </c>
       <c r="M16">
-        <v>19.96062992125984</v>
+        <v>14.45631678189818</v>
       </c>
       <c r="N16">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O16">
-        <v>0.009446438692612885</v>
+        <v>0.0003919124937783891</v>
       </c>
       <c r="P16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q16">
-        <v>0</v>
+        <v>0.04074979625101875</v>
       </c>
       <c r="R16">
         <v>0</v>
@@ -1440,58 +1440,58 @@
         <v>34</v>
       </c>
       <c r="B17">
-        <v>33976</v>
+        <v>2468</v>
       </c>
       <c r="C17">
-        <v>4947</v>
+        <v>353</v>
       </c>
       <c r="D17">
-        <v>9816</v>
+        <v>706</v>
       </c>
       <c r="E17">
-        <v>143.0427360489757</v>
+        <v>30.46839546191248</v>
       </c>
       <c r="F17">
-        <v>135.3796240145543</v>
+        <v>28.72804532577904</v>
       </c>
       <c r="G17">
-        <v>140.4318459657702</v>
+        <v>32.78895184135978</v>
       </c>
       <c r="H17">
-        <v>247</v>
+        <v>479</v>
       </c>
       <c r="I17">
-        <v>0.005082283612001597</v>
+        <v>0.6370019681897974</v>
       </c>
       <c r="J17">
-        <v>253</v>
+        <v>527</v>
       </c>
       <c r="K17">
-        <v>0.0377768122044487</v>
+        <v>5.196726161128094</v>
       </c>
       <c r="L17">
-        <v>237</v>
+        <v>572</v>
       </c>
       <c r="M17">
-        <v>0.01719286256809135</v>
+        <v>2.470949069074258</v>
       </c>
       <c r="N17">
-        <v>680</v>
+        <v>624</v>
       </c>
       <c r="O17">
-        <v>0.0139917119682635</v>
+        <v>0.8298313740092558</v>
       </c>
       <c r="P17">
-        <v>89</v>
+        <v>76</v>
       </c>
       <c r="Q17">
-        <v>0.01328907623002346</v>
+        <v>0.749432994773691</v>
       </c>
       <c r="R17">
-        <v>254</v>
+        <v>147</v>
       </c>
       <c r="S17">
-        <v>0.01842610587466331</v>
+        <v>0.6350166313879648</v>
       </c>
     </row>
     <row r="18" spans="1:19">
@@ -1617,58 +1617,58 @@
         <v>37</v>
       </c>
       <c r="B20">
-        <v>502</v>
+        <v>595</v>
       </c>
       <c r="C20">
-        <v>72</v>
+        <v>85</v>
       </c>
       <c r="D20">
-        <v>145</v>
+        <v>171</v>
       </c>
       <c r="E20">
-        <v>51.05577689243028</v>
+        <v>54.32100840336135</v>
       </c>
       <c r="F20">
-        <v>65.27777777777777</v>
+        <v>52.83529411764706</v>
       </c>
       <c r="G20">
-        <v>49.98620689655172</v>
+        <v>57.8187134502924</v>
       </c>
       <c r="H20">
-        <v>896</v>
+        <v>1195</v>
       </c>
       <c r="I20">
-        <v>3.495903238392509</v>
+        <v>3.697286593855388</v>
       </c>
       <c r="J20">
-        <v>493</v>
+        <v>588</v>
       </c>
       <c r="K20">
-        <v>10.48936170212766</v>
+        <v>13.09285237140949</v>
       </c>
       <c r="L20">
-        <v>573</v>
+        <v>807</v>
       </c>
       <c r="M20">
-        <v>7.905629139072848</v>
+        <v>8.162233235561848</v>
       </c>
       <c r="N20">
-        <v>206</v>
+        <v>235</v>
       </c>
       <c r="O20">
-        <v>0.8037456106125634</v>
+        <v>0.727081464063612</v>
       </c>
       <c r="P20">
-        <v>48</v>
+        <v>30</v>
       </c>
       <c r="Q20">
-        <v>1.021276595744681</v>
+        <v>0.6680026720106881</v>
       </c>
       <c r="R20">
-        <v>59</v>
+        <v>108</v>
       </c>
       <c r="S20">
-        <v>0.8140176600441501</v>
+        <v>1.092343481339132</v>
       </c>
     </row>
   </sheetData>

</xml_diff>